<commit_message>
fix bug in get_mapping_df() (was incorrectly dropping some rows). update dummy data and tests for this
</commit_message>
<xml_diff>
--- a/inst/extdata/dummy_all_lkps_maps_v3.xlsx
+++ b/inst/extdata/dummy_all_lkps_maps_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alasdair/Documents/phd/r_packages/codemapper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492C8C4E-1ADE-B242-A839-88A12CDFA3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CDDD80-006A-4F4F-A453-2BECEBA9F5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="13" r:id="rId1"/>
@@ -36,17 +36,27 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">read_v2_lkp!$A$1:$C$25</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2833" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="896">
   <si>
     <t>BNF_Presentation_Code</t>
   </si>
@@ -2897,6 +2907,33 @@
   <si>
     <t>**DUMMY DATA** Coding system lookups and mappings
 Version 3 (May 2021)</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>J5310</t>
+  </si>
+  <si>
+    <t>Sub-mucosal anal fistula</t>
+  </si>
+  <si>
+    <t>J5311</t>
+  </si>
+  <si>
+    <t>Y30FJ</t>
+  </si>
+  <si>
+    <t>Intersphincteric fistula</t>
+  </si>
+  <si>
+    <t>Y30FL</t>
+  </si>
+  <si>
+    <t>Submucosal anal fistula</t>
+  </si>
+  <si>
+    <t>Inter-muscular anal fistula</t>
   </si>
 </sst>
 </file>
@@ -3672,7 +3709,15 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5940,7 +5985,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
-    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5951,7 +5996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -7136,7 +7181,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C108">
-    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7227,10 +7272,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7627,14 +7672,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>887</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>888</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>889</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>889</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>891</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>892</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>887</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>888</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>889</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>889</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>893</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>894</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>887</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>895</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>895</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>891</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>892</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>887</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>895</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>895</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>893</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>894</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>863</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K13">
-    <sortCondition sortBy="cellColor" ref="C2:C13" dxfId="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K17">
+    <sortCondition sortBy="cellColor" ref="C2:C17" dxfId="1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15615,7 +15800,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L150">
-    <sortCondition sortBy="cellColor" ref="A19:A150" dxfId="5"/>
+    <sortCondition sortBy="cellColor" ref="A19:A150" dxfId="6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -16141,7 +16326,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
-    <sortCondition sortBy="cellColor" ref="A3:A41" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="A3:A41" dxfId="5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16420,7 +16605,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
-    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
various updates to caliber-realted functions/tests
</commit_message>
<xml_diff>
--- a/inst/extdata/dummy_all_lkps_maps_v3.xlsx
+++ b/inst/extdata/dummy_all_lkps_maps_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alasdair/Documents/phd/r_packages/codemapper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CDDD80-006A-4F4F-A453-2BECEBA9F5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA438AC-1557-0041-B323-D1BF5BAC814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="13" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3199" uniqueCount="964">
   <si>
     <t>BNF_Presentation_Code</t>
   </si>
@@ -2934,6 +2934,210 @@
   </si>
   <si>
     <t>Inter-muscular anal fistula</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>K05..</t>
+  </si>
+  <si>
+    <t>Chronic renal failure</t>
+  </si>
+  <si>
+    <t>End stage renal failure</t>
+  </si>
+  <si>
+    <t>X30J0</t>
+  </si>
+  <si>
+    <t>Y31gA</t>
+  </si>
+  <si>
+    <t>K050.</t>
+  </si>
+  <si>
+    <t>K0D..</t>
+  </si>
+  <si>
+    <t>End-stage renal disease</t>
+  </si>
+  <si>
+    <t>Y31gC</t>
+  </si>
+  <si>
+    <t>End stage renal disease</t>
+  </si>
+  <si>
+    <t>ESRF - End stage renal failure</t>
+  </si>
+  <si>
+    <t>ESRD - End stage renal disease</t>
+  </si>
+  <si>
+    <t>ESCRF - End stage chronic renal failure</t>
+  </si>
+  <si>
+    <t>End stage chronc renal failure</t>
+  </si>
+  <si>
+    <t>Xa0lK</t>
+  </si>
+  <si>
+    <t>Diabetic (femoral mononeuropathy) &amp; (Diabetic amyotrophy)</t>
+  </si>
+  <si>
+    <t>Diabetic femoral mononeuropathy</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus with neurological manifestation</t>
+  </si>
+  <si>
+    <t>XE10H</t>
+  </si>
+  <si>
+    <t>Y41Oy</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus with neuropathy</t>
+  </si>
+  <si>
+    <t>X00Ag</t>
+  </si>
+  <si>
+    <t>Y00Xb</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus with polyneuropathy</t>
+  </si>
+  <si>
+    <t>XE15k</t>
+  </si>
+  <si>
+    <t>Y00Xg</t>
+  </si>
+  <si>
+    <t>Diabetic amyotrophy</t>
+  </si>
+  <si>
+    <t>Y00Xo</t>
+  </si>
+  <si>
+    <t>XaPmX</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F3813</t>
+  </si>
+  <si>
+    <t>Myasthenic syndrome due to diabetic amyotrophy</t>
+  </si>
+  <si>
+    <t>XE15n</t>
+  </si>
+  <si>
+    <t>Ya25o</t>
+  </si>
+  <si>
+    <t>X00AG</t>
+  </si>
+  <si>
+    <t>Autosomal dominant sensory neuropathy</t>
+  </si>
+  <si>
+    <t>Hereditary sensory and autonomic neuropathy type I</t>
+  </si>
+  <si>
+    <t>Polyneuropathy in diabetes</t>
+  </si>
+  <si>
+    <t>Diabetic neuropathy</t>
+  </si>
+  <si>
+    <t>F48</t>
+  </si>
+  <si>
+    <t>Other neurotic disorders</t>
+  </si>
+  <si>
+    <t>F48.0</t>
+  </si>
+  <si>
+    <t>F480</t>
+  </si>
+  <si>
+    <t>Neurasthenia</t>
+  </si>
+  <si>
+    <t>F48.1</t>
+  </si>
+  <si>
+    <t>F481</t>
+  </si>
+  <si>
+    <t>Depersonalization-derealization syndrome</t>
+  </si>
+  <si>
+    <t>J45</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>J45.0</t>
+  </si>
+  <si>
+    <t>J450</t>
+  </si>
+  <si>
+    <t>Predominantly allergic asthma</t>
+  </si>
+  <si>
+    <t>J45.1</t>
+  </si>
+  <si>
+    <t>J451</t>
+  </si>
+  <si>
+    <t>Nonallergic asthma</t>
+  </si>
+  <si>
+    <t>J45.8</t>
+  </si>
+  <si>
+    <t>J458</t>
+  </si>
+  <si>
+    <t>Mixed asthma</t>
+  </si>
+  <si>
+    <t>J45.9</t>
+  </si>
+  <si>
+    <t>J459</t>
+  </si>
+  <si>
+    <t>Asthma, unspecified</t>
+  </si>
+  <si>
+    <t>4930</t>
+  </si>
+  <si>
+    <t>EXTRINSIC ASTHMA</t>
+  </si>
+  <si>
+    <t>4939</t>
+  </si>
+  <si>
+    <t>ASTHMA, UNSPECIFIED</t>
+  </si>
+  <si>
+    <t>4931</t>
+  </si>
+  <si>
+    <t>INTRINSIC ASTHMA</t>
   </si>
 </sst>
 </file>
@@ -3709,7 +3913,63 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5985,7 +6245,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
-    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7181,7 +7441,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C108">
-    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7272,10 +7532,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7322,178 +7582,178 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="12" t="s">
+        <v>915</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>916</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>917</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="K2" s="15">
+      <c r="G3" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>919</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>917</v>
+      </c>
+      <c r="K3" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="B4" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>921</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>922</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>911</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>925</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="K3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="K4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="K5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>571</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="K6" s="15">
+      <c r="J6" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="K6" s="12">
         <v>1</v>
       </c>
     </row>
@@ -7508,25 +7768,25 @@
         <v>378</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>466</v>
+        <v>378</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>35</v>
+        <v>568</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>228</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="K7" s="15">
         <v>1</v>
@@ -7537,13 +7797,13 @@
         <v>111</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>467</v>
+        <v>378</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>467</v>
+        <v>378</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>568</v>
@@ -7555,16 +7815,16 @@
         <v>228</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K8" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -7572,16 +7832,16 @@
         <v>111</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>467</v>
+        <v>378</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>378</v>
+        <v>540</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>34</v>
+        <v>569</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>358</v>
@@ -7590,13 +7850,13 @@
         <v>228</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>358</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K9" s="15">
         <v>1</v>
@@ -7607,16 +7867,16 @@
         <v>111</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>467</v>
+        <v>378</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>378</v>
+        <v>540</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>34</v>
+        <v>569</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>358</v>
@@ -7642,16 +7902,16 @@
         <v>111</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>467</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>466</v>
-      </c>
       <c r="E11" s="15" t="s">
-        <v>569</v>
+        <v>34</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>358</v>
@@ -7660,166 +7920,586 @@
         <v>228</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K11" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="K12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="K13" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="K14" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="K16" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>926</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>927</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>929</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>930</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>926</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>927</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>911</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>926</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>927</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>925</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="K19" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>889</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>889</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H20" s="12" t="s">
         <v>891</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I20" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J20" s="12" t="s">
         <v>892</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K20" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+    <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>889</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>889</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H21" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I21" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J21" s="12" t="s">
         <v>894</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K21" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+    <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>895</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>895</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H22" s="12" t="s">
         <v>891</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I22" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J22" s="12" t="s">
         <v>892</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K22" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>895</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>895</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H23" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I23" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J23" s="12" t="s">
         <v>894</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K23" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+    <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>896</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>897</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>898</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>900</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>901</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="K24" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>896</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>902</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>900</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>901</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="K25" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>896</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>903</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>900</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>901</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>896</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>903</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>900</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>905</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>906</v>
+      </c>
+      <c r="K27" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
         <v>863</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K17">
-    <sortCondition sortBy="cellColor" ref="C2:C17" dxfId="1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K29">
+    <sortCondition sortBy="cellColor" ref="C7:C29" dxfId="8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7828,10 +8508,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7927,8 +8607,260 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>900</v>
+      </c>
+      <c r="B7" t="s">
+        <v>899</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>900</v>
+      </c>
+      <c r="B8" t="s">
+        <v>907</v>
+      </c>
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>900</v>
+      </c>
+      <c r="B9" t="s">
+        <v>906</v>
+      </c>
+      <c r="C9" t="s">
+        <v>358</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>900</v>
+      </c>
+      <c r="B10" t="s">
+        <v>908</v>
+      </c>
+      <c r="C10" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>900</v>
+      </c>
+      <c r="B11" t="s">
+        <v>909</v>
+      </c>
+      <c r="C11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>900</v>
+      </c>
+      <c r="B12" t="s">
+        <v>910</v>
+      </c>
+      <c r="C12" t="s">
+        <v>358</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>911</v>
+      </c>
+      <c r="B13" t="s">
+        <v>912</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>911</v>
+      </c>
+      <c r="B14" t="s">
+        <v>913</v>
+      </c>
+      <c r="C14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>915</v>
+      </c>
+      <c r="B15" t="s">
+        <v>914</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>931</v>
+      </c>
+      <c r="B16" t="s">
+        <v>932</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>931</v>
+      </c>
+      <c r="B17" t="s">
+        <v>933</v>
+      </c>
+      <c r="C17" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>918</v>
+      </c>
+      <c r="B18" t="s">
+        <v>935</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>918</v>
+      </c>
+      <c r="B19" t="s">
+        <v>917</v>
+      </c>
+      <c r="C19" t="s">
+        <v>358</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>921</v>
+      </c>
+      <c r="B20" t="s">
+        <v>430</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>921</v>
+      </c>
+      <c r="B21" t="s">
+        <v>920</v>
+      </c>
+      <c r="C21" t="s">
+        <v>358</v>
+      </c>
+      <c r="D21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>921</v>
+      </c>
+      <c r="B22" t="s">
+        <v>934</v>
+      </c>
+      <c r="C22" t="s">
+        <v>358</v>
+      </c>
+      <c r="D22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>925</v>
+      </c>
+      <c r="B23" t="s">
+        <v>923</v>
+      </c>
+      <c r="C23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>929</v>
+      </c>
+      <c r="B24" t="s">
+        <v>928</v>
+      </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
         <v>863</v>
       </c>
     </row>
@@ -9962,10 +10894,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10132,22 +11064,46 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>210</v>
+        <v>958</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>650</v>
+        <v>959</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
+        <v>962</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>865</v>
       </c>
     </row>
@@ -10158,10 +11114,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L150"/>
+  <dimension ref="A1:L158"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:XFD101"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131:XFD135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14009,19 +14965,19 @@
     </row>
     <row r="102" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
-        <v>502</v>
+        <v>936</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>347</v>
+        <v>936</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D102" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>636</v>
+        <v>937</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>678</v>
@@ -14047,19 +15003,19 @@
     </row>
     <row r="103" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
-        <v>789</v>
+        <v>938</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>790</v>
+        <v>939</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D103" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>465</v>
+        <v>940</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>678</v>
@@ -14085,19 +15041,19 @@
     </row>
     <row r="104" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
-        <v>791</v>
+        <v>941</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>504</v>
+        <v>942</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D104" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>430</v>
+        <v>943</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>678</v>
@@ -14123,10 +15079,10 @@
     </row>
     <row r="105" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
-        <v>792</v>
+        <v>502</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>793</v>
+        <v>347</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>723</v>
@@ -14135,7 +15091,7 @@
         <v>2</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>678</v>
@@ -14161,10 +15117,10 @@
     </row>
     <row r="106" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>723</v>
@@ -14173,7 +15129,7 @@
         <v>2</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>432</v>
+        <v>465</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>678</v>
@@ -14199,10 +15155,10 @@
     </row>
     <row r="107" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>797</v>
+        <v>504</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>723</v>
@@ -14211,7 +15167,7 @@
         <v>2</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>678</v>
@@ -14237,19 +15193,19 @@
     </row>
     <row r="108" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>327</v>
+        <v>793</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D108" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>678</v>
@@ -14275,19 +15231,19 @@
     </row>
     <row r="109" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
-        <v>329</v>
+        <v>794</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>329</v>
+        <v>795</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D109" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>678</v>
@@ -14313,19 +15269,19 @@
     </row>
     <row r="110" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>335</v>
+        <v>797</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D110" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>642</v>
+        <v>431</v>
       </c>
       <c r="F110" s="12" t="s">
         <v>678</v>
@@ -14351,10 +15307,10 @@
     </row>
     <row r="111" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>677</v>
@@ -14363,7 +15319,7 @@
         <v>3</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>801</v>
+        <v>639</v>
       </c>
       <c r="F111" s="12" t="s">
         <v>678</v>
@@ -14389,10 +15345,10 @@
     </row>
     <row r="112" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>677</v>
@@ -14401,7 +15357,7 @@
         <v>3</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F112" s="12" t="s">
         <v>678</v>
@@ -14427,10 +15383,10 @@
     </row>
     <row r="113" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>677</v>
@@ -14439,7 +15395,7 @@
         <v>3</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>439</v>
+        <v>642</v>
       </c>
       <c r="F113" s="12" t="s">
         <v>678</v>
@@ -14465,10 +15421,10 @@
     </row>
     <row r="114" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>677</v>
@@ -14477,7 +15433,7 @@
         <v>3</v>
       </c>
       <c r="E114" s="12" t="s">
-        <v>643</v>
+        <v>801</v>
       </c>
       <c r="F114" s="12" t="s">
         <v>678</v>
@@ -14503,10 +15459,10 @@
     </row>
     <row r="115" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>677</v>
@@ -14515,7 +15471,7 @@
         <v>3</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F115" s="12" t="s">
         <v>678</v>
@@ -14541,10 +15497,10 @@
     </row>
     <row r="116" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>677</v>
@@ -14553,7 +15509,7 @@
         <v>3</v>
       </c>
       <c r="E116" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F116" s="12" t="s">
         <v>678</v>
@@ -14579,10 +15535,10 @@
     </row>
     <row r="117" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>677</v>
@@ -14591,7 +15547,7 @@
         <v>3</v>
       </c>
       <c r="E117" s="12" t="s">
-        <v>442</v>
+        <v>643</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>678</v>
@@ -14617,10 +15573,10 @@
     </row>
     <row r="118" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
-        <v>806</v>
+        <v>331</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>677</v>
@@ -14629,7 +15585,7 @@
         <v>3</v>
       </c>
       <c r="E118" s="12" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>678</v>
@@ -14655,10 +15611,10 @@
     </row>
     <row r="119" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>677</v>
@@ -14667,7 +15623,7 @@
         <v>3</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>644</v>
+        <v>441</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>678</v>
@@ -14693,10 +15649,10 @@
     </row>
     <row r="120" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
-        <v>345</v>
+        <v>805</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>677</v>
@@ -14705,7 +15661,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>678</v>
@@ -14731,10 +15687,10 @@
     </row>
     <row r="121" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C121" s="12" t="s">
         <v>677</v>
@@ -14743,7 +15699,7 @@
         <v>3</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
       <c r="F121" s="12" t="s">
         <v>678</v>
@@ -14769,10 +15725,10 @@
     </row>
     <row r="122" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>677</v>
@@ -14781,7 +15737,7 @@
         <v>3</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F122" s="12" t="s">
         <v>678</v>
@@ -14807,10 +15763,10 @@
     </row>
     <row r="123" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
-        <v>810</v>
+        <v>345</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C123" s="12" t="s">
         <v>677</v>
@@ -14819,7 +15775,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F123" s="12" t="s">
         <v>678</v>
@@ -14845,10 +15801,10 @@
     </row>
     <row r="124" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>231</v>
+        <v>338</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>677</v>
@@ -14857,7 +15813,7 @@
         <v>3</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>646</v>
+        <v>476</v>
       </c>
       <c r="F124" s="12" t="s">
         <v>678</v>
@@ -14883,10 +15839,10 @@
     </row>
     <row r="125" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>677</v>
@@ -14895,7 +15851,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="12" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F125" s="12" t="s">
         <v>678</v>
@@ -14921,19 +15877,19 @@
     </row>
     <row r="126" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>814</v>
+        <v>346</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D126" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E126" s="12" t="s">
-        <v>648</v>
+        <v>445</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>678</v>
@@ -14959,10 +15915,10 @@
     </row>
     <row r="127" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>677</v>
@@ -14971,7 +15927,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="12" t="s">
-        <v>364</v>
+        <v>646</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>678</v>
@@ -14997,19 +15953,19 @@
     </row>
     <row r="128" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="s">
-        <v>837</v>
+        <v>812</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>505</v>
+        <v>344</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D128" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="F128" s="12" t="s">
         <v>678</v>
@@ -15035,10 +15991,10 @@
     </row>
     <row r="129" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>723</v>
@@ -15047,7 +16003,7 @@
         <v>2</v>
       </c>
       <c r="E129" s="12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F129" s="12" t="s">
         <v>678</v>
@@ -15073,343 +16029,343 @@
     </row>
     <row r="130" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="s">
+        <v>815</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D130" s="12">
+        <v>3</v>
+      </c>
+      <c r="E130" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="F130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K130" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L130" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="12" t="s">
+        <v>944</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>944</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D131" s="12">
+        <v>3</v>
+      </c>
+      <c r="E131" s="12" t="s">
+        <v>945</v>
+      </c>
+      <c r="F131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K131" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L131" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="12" t="s">
+        <v>946</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>947</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D132" s="12">
+        <v>3</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>948</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L132" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="12" t="s">
+        <v>949</v>
+      </c>
+      <c r="B133" s="12" t="s">
+        <v>950</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D133" s="12">
+        <v>3</v>
+      </c>
+      <c r="E133" s="12" t="s">
+        <v>951</v>
+      </c>
+      <c r="F133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L133" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="12" t="s">
+        <v>952</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>953</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D134" s="12">
+        <v>3</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>954</v>
+      </c>
+      <c r="F134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K134" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L134" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="12" t="s">
+        <v>955</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>956</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D135" s="12">
+        <v>3</v>
+      </c>
+      <c r="E135" s="12" t="s">
+        <v>957</v>
+      </c>
+      <c r="F135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K135" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L135" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="12" t="s">
+        <v>837</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="D136" s="12">
+        <v>2</v>
+      </c>
+      <c r="E136" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="F136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K136" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L136" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="12" t="s">
+        <v>821</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>822</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="D137" s="12">
+        <v>2</v>
+      </c>
+      <c r="E137" s="12" t="s">
+        <v>649</v>
+      </c>
+      <c r="F137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K137" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L137" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="12" t="s">
         <v>823</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B138" s="12" t="s">
         <v>824</v>
       </c>
-      <c r="C130" s="12" t="s">
+      <c r="C138" s="12" t="s">
         <v>723</v>
       </c>
-      <c r="D130" s="12">
+      <c r="D138" s="12">
         <v>2</v>
       </c>
-      <c r="E130" s="12" t="s">
+      <c r="E138" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="F130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K130" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L130" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A131" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B131" s="17" t="s">
-        <v>826</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D131" s="17">
-        <v>2</v>
-      </c>
-      <c r="E131" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="H131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K131" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L131" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A132" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B132" s="17" t="s">
-        <v>827</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D132" s="17">
-        <v>2</v>
-      </c>
-      <c r="E132" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F132" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G132" s="17" t="s">
-        <v>816</v>
-      </c>
-      <c r="H132" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I132" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J132" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K132" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L132" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A133" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B133" s="17" t="s">
-        <v>828</v>
-      </c>
-      <c r="C133" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D133" s="17">
-        <v>2</v>
-      </c>
-      <c r="E133" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F133" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G133" s="17" t="s">
-        <v>478</v>
-      </c>
-      <c r="H133" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I133" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J133" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K133" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L133" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A134" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B134" s="17" t="s">
-        <v>829</v>
-      </c>
-      <c r="C134" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D134" s="17">
-        <v>2</v>
-      </c>
-      <c r="E134" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F134" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G134" s="17" t="s">
-        <v>479</v>
-      </c>
-      <c r="H134" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I134" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J134" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K134" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L134" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A135" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B135" s="17" t="s">
-        <v>830</v>
-      </c>
-      <c r="C135" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D135" s="17">
-        <v>2</v>
-      </c>
-      <c r="E135" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F135" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G135" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="H135" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I135" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J135" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K135" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L135" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A136" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B136" s="17" t="s">
-        <v>831</v>
-      </c>
-      <c r="C136" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D136" s="17">
-        <v>2</v>
-      </c>
-      <c r="E136" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F136" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G136" s="17" t="s">
-        <v>481</v>
-      </c>
-      <c r="H136" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I136" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J136" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K136" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L136" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A137" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B137" s="17" t="s">
-        <v>832</v>
-      </c>
-      <c r="C137" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D137" s="17">
-        <v>2</v>
-      </c>
-      <c r="E137" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F137" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G137" s="17" t="s">
-        <v>817</v>
-      </c>
-      <c r="H137" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I137" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J137" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K137" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L137" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A138" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B138" s="17" t="s">
-        <v>833</v>
-      </c>
-      <c r="C138" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D138" s="17">
-        <v>2</v>
-      </c>
-      <c r="E138" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F138" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G138" s="17" t="s">
-        <v>477</v>
-      </c>
-      <c r="H138" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I138" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J138" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K138" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L138" s="17" t="s">
+      <c r="F138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L138" s="12" t="s">
         <v>678</v>
       </c>
     </row>
@@ -15418,7 +16374,7 @@
         <v>825</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="C139" s="17" t="s">
         <v>723</v>
@@ -15433,7 +16389,7 @@
         <v>678</v>
       </c>
       <c r="G139" s="17" t="s">
-        <v>818</v>
+        <v>678</v>
       </c>
       <c r="H139" s="17" t="s">
         <v>678</v>
@@ -15456,7 +16412,7 @@
         <v>825</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="C140" s="17" t="s">
         <v>723</v>
@@ -15471,7 +16427,7 @@
         <v>678</v>
       </c>
       <c r="G140" s="17" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="H140" s="17" t="s">
         <v>678</v>
@@ -15494,7 +16450,7 @@
         <v>825</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="C141" s="17" t="s">
         <v>723</v>
@@ -15509,298 +16465,602 @@
         <v>678</v>
       </c>
       <c r="G141" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="H141" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I141" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J141" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K141" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L141" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A142" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B142" s="17" t="s">
+        <v>829</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D142" s="17">
+        <v>2</v>
+      </c>
+      <c r="E142" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F142" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G142" s="17" t="s">
+        <v>479</v>
+      </c>
+      <c r="H142" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I142" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J142" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K142" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L142" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A143" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B143" s="17" t="s">
+        <v>830</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D143" s="17">
+        <v>2</v>
+      </c>
+      <c r="E143" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F143" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G143" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="H143" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I143" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J143" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K143" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L143" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A144" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B144" s="17" t="s">
+        <v>831</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D144" s="17">
+        <v>2</v>
+      </c>
+      <c r="E144" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F144" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G144" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="H144" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I144" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J144" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K144" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L144" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A145" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B145" s="17" t="s">
+        <v>832</v>
+      </c>
+      <c r="C145" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D145" s="17">
+        <v>2</v>
+      </c>
+      <c r="E145" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F145" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G145" s="17" t="s">
+        <v>817</v>
+      </c>
+      <c r="H145" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I145" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J145" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K145" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L145" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A146" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>833</v>
+      </c>
+      <c r="C146" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D146" s="17">
+        <v>2</v>
+      </c>
+      <c r="E146" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F146" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G146" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="H146" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I146" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J146" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K146" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L146" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A147" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>834</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D147" s="17">
+        <v>2</v>
+      </c>
+      <c r="E147" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F147" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G147" s="17" t="s">
+        <v>818</v>
+      </c>
+      <c r="H147" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I147" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J147" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K147" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L147" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A148" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B148" s="17" t="s">
+        <v>835</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D148" s="17">
+        <v>2</v>
+      </c>
+      <c r="E148" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F148" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G148" s="17" t="s">
+        <v>819</v>
+      </c>
+      <c r="H148" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I148" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J148" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K148" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L148" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A149" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>836</v>
+      </c>
+      <c r="C149" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D149" s="17">
+        <v>2</v>
+      </c>
+      <c r="E149" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G149" s="17" t="s">
         <v>820</v>
       </c>
-      <c r="H141" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I141" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J141" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K141" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L141" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="12" t="s">
+      <c r="H149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L149" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="B142" s="12" t="s">
+      <c r="B150" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="C142" s="12" t="s">
+      <c r="C150" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D142" s="12">
+      <c r="D150" s="12">
         <v>3</v>
       </c>
-      <c r="E142" s="12" t="s">
+      <c r="E150" s="12" t="s">
         <v>838</v>
       </c>
-      <c r="F142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K142" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L142" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="12" t="s">
+      <c r="F150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K150" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L150" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="12" t="s">
         <v>839</v>
       </c>
-      <c r="B143" s="12" t="s">
+      <c r="B151" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="C143" s="12" t="s">
+      <c r="C151" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D143" s="12">
+      <c r="D151" s="12">
         <v>3</v>
       </c>
-      <c r="E143" s="12" t="s">
+      <c r="E151" s="12" t="s">
         <v>840</v>
       </c>
-      <c r="F143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K143" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L143" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="12" t="s">
+      <c r="F151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K151" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L151" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="12" t="s">
         <v>841</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B152" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="C144" s="12" t="s">
+      <c r="C152" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D144" s="12">
+      <c r="D152" s="12">
         <v>3</v>
       </c>
-      <c r="E144" s="12" t="s">
+      <c r="E152" s="12" t="s">
         <v>842</v>
       </c>
-      <c r="F144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K144" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L144" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="12" t="s">
+      <c r="F152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K152" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L152" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="12" t="s">
         <v>843</v>
       </c>
-      <c r="B145" s="12" t="s">
+      <c r="B153" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="C145" s="12" t="s">
+      <c r="C153" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D145" s="12">
+      <c r="D153" s="12">
         <v>3</v>
       </c>
-      <c r="E145" s="12" t="s">
+      <c r="E153" s="12" t="s">
         <v>844</v>
       </c>
-      <c r="F145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K145" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L145" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="12" t="s">
+      <c r="F153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K153" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L153" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="12" t="s">
         <v>845</v>
       </c>
-      <c r="B146" s="12" t="s">
+      <c r="B154" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="C146" s="12" t="s">
+      <c r="C154" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D146" s="12">
+      <c r="D154" s="12">
         <v>3</v>
       </c>
-      <c r="E146" s="12" t="s">
+      <c r="E154" s="12" t="s">
         <v>846</v>
       </c>
-      <c r="F146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K146" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L146" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="12" t="s">
+      <c r="F154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K154" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L154" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="12" t="s">
         <v>847</v>
       </c>
-      <c r="B147" s="12" t="s">
+      <c r="B155" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="C147" s="12" t="s">
+      <c r="C155" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D147" s="12">
+      <c r="D155" s="12">
         <v>3</v>
       </c>
-      <c r="E147" s="12" t="s">
+      <c r="E155" s="12" t="s">
         <v>848</v>
       </c>
-      <c r="F147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K147" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L147" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="12" t="s">
+      <c r="F155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L155" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="12" t="s">
         <v>849</v>
       </c>
-      <c r="B148" s="12" t="s">
+      <c r="B156" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="C148" s="12" t="s">
+      <c r="C156" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="D148" s="12">
+      <c r="D156" s="12">
         <v>3</v>
       </c>
-      <c r="E148" s="12" t="s">
+      <c r="E156" s="12" t="s">
         <v>850</v>
       </c>
-      <c r="F148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K148" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L148" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A150" s="18" t="s">
+      <c r="F156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L156" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A158" s="18" t="s">
         <v>862</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L150">
-    <sortCondition sortBy="cellColor" ref="A19:A150" dxfId="6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L158">
+    <sortCondition sortBy="cellColor" ref="A19:A158" dxfId="13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -15809,10 +17069,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A22" sqref="A22:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16094,239 +17354,379 @@
         <v>639</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>651</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
-        <v>589</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D31" s="17"/>
+    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>958</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>959</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>947</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>961</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>947</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>958</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>959</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>950</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>962</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>950</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>958</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>959</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>953</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>962</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>953</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>961</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>953</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>958</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>959</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>956</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>962</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>956</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>961</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>956</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>957</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>590</v>
+        <v>210</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D32" s="17"/>
+        <v>255</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>591</v>
+        <v>220</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D33" s="17"/>
+        <v>255</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D34" s="17"/>
+        <v>234</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D35" s="17"/>
+        <v>291</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D36" s="17"/>
+        <v>313</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="D37" s="17"/>
+        <v>240</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D40" s="17"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D44" s="17"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D46" s="17"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="D47" s="17"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B48" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C48" s="17" t="s">
         <v>576</v>
       </c>
-      <c r="D38" s="17"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="D48" s="17"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
         <v>865</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
-    <sortCondition sortBy="cellColor" ref="A3:A41" dxfId="5"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D51">
+    <sortCondition sortBy="cellColor" ref="A3:A51" dxfId="12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16605,7 +18005,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
-    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add to inst/extdata dummy data, including phecode files
</commit_message>
<xml_diff>
--- a/inst/extdata/dummy_all_lkps_maps_v3.xlsx
+++ b/inst/extdata/dummy_all_lkps_maps_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alasdair/Documents/phd/r_packages/codemapper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA438AC-1557-0041-B323-D1BF5BAC814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF5310-3424-B140-B251-2C0C3B560CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="read_ctv3_read_v2" sheetId="15" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">read_v2_lkp!$A$1:$C$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">read_v2_lkp!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3199" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="996">
   <si>
     <t>BNF_Presentation_Code</t>
   </si>
@@ -3138,6 +3138,102 @@
   </si>
   <si>
     <t>INTRINSIC ASTHMA</t>
+  </si>
+  <si>
+    <t>P700</t>
+  </si>
+  <si>
+    <t>P701</t>
+  </si>
+  <si>
+    <t>P702</t>
+  </si>
+  <si>
+    <t>XaIP9</t>
+  </si>
+  <si>
+    <t>L721</t>
+  </si>
+  <si>
+    <t>H028</t>
+  </si>
+  <si>
+    <t>N508</t>
+  </si>
+  <si>
+    <t>N608</t>
+  </si>
+  <si>
+    <t>N948</t>
+  </si>
+  <si>
+    <t>Sebaceous cyst</t>
+  </si>
+  <si>
+    <t>Keratinising cyst</t>
+  </si>
+  <si>
+    <t>Keratinous cyst</t>
+  </si>
+  <si>
+    <t>Wen</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus</t>
+  </si>
+  <si>
+    <t>DM - Diabetes mellitus</t>
+  </si>
+  <si>
+    <t>L72.1</t>
+  </si>
+  <si>
+    <t>Trichilemmal cyst</t>
+  </si>
+  <si>
+    <t>H02.8</t>
+  </si>
+  <si>
+    <t>Other specified disorders of eyelid</t>
+  </si>
+  <si>
+    <t>N50.8</t>
+  </si>
+  <si>
+    <t>Other specified disorders of male genital organs</t>
+  </si>
+  <si>
+    <t>N60.8</t>
+  </si>
+  <si>
+    <t>Other benign mammary dysplasias</t>
+  </si>
+  <si>
+    <t>N94.8</t>
+  </si>
+  <si>
+    <t>Other specified conditions associated with female genital organs and menstrual cycle</t>
+  </si>
+  <si>
+    <t>O24.9</t>
+  </si>
+  <si>
+    <t>P70.0</t>
+  </si>
+  <si>
+    <t>Syndrome of infant of mother with gestational diabetes</t>
+  </si>
+  <si>
+    <t>P70.1</t>
+  </si>
+  <si>
+    <t>Syndrome of infant of a diabetic mother</t>
+  </si>
+  <si>
+    <t>P70.2</t>
+  </si>
+  <si>
+    <t>Neonatal diabetes mellitus</t>
   </si>
 </sst>
 </file>
@@ -3913,55 +4009,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6245,7 +6293,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
-    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="10"/>
+    <sortCondition sortBy="cellColor" ref="A2:A122" dxfId="4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6256,7 +6304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -7441,7 +7489,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C108">
-    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="9"/>
+    <sortCondition sortBy="cellColor" ref="A2:A108" dxfId="3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8499,7 +8547,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K29">
-    <sortCondition sortBy="cellColor" ref="C7:C29" dxfId="8"/>
+    <sortCondition sortBy="cellColor" ref="C7:C29" dxfId="2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8508,10 +8556,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8537,31 +8585,31 @@
         <v>884</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>466</v>
-      </c>
-      <c r="C2" s="18" t="s">
+    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>977</v>
+      </c>
+      <c r="C2" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>467</v>
-      </c>
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>978</v>
+      </c>
+      <c r="C3" t="s">
         <v>358</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8570,10 +8618,10 @@
         <v>228</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>111</v>
@@ -8584,7 +8632,7 @@
         <v>228</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>358</v>
@@ -8598,7 +8646,7 @@
         <v>228</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>358</v>
@@ -8607,31 +8655,31 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>900</v>
-      </c>
-      <c r="B7" t="s">
-        <v>899</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>900</v>
-      </c>
-      <c r="B8" t="s">
-        <v>907</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>470</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="18" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8640,10 +8688,10 @@
         <v>900</v>
       </c>
       <c r="B9" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="C9" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
         <v>111</v>
@@ -8654,7 +8702,7 @@
         <v>900</v>
       </c>
       <c r="B10" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C10" t="s">
         <v>358</v>
@@ -8668,7 +8716,7 @@
         <v>900</v>
       </c>
       <c r="B11" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="C11" t="s">
         <v>358</v>
@@ -8682,7 +8730,7 @@
         <v>900</v>
       </c>
       <c r="B12" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C12" t="s">
         <v>358</v>
@@ -8693,13 +8741,13 @@
     </row>
     <row r="13" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>911</v>
+        <v>900</v>
       </c>
       <c r="B13" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="D13" t="s">
         <v>111</v>
@@ -8707,10 +8755,10 @@
     </row>
     <row r="14" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>911</v>
+        <v>900</v>
       </c>
       <c r="B14" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="C14" t="s">
         <v>358</v>
@@ -8721,10 +8769,10 @@
     </row>
     <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="B15" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C15" t="s">
         <v>115</v>
@@ -8735,13 +8783,13 @@
     </row>
     <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>931</v>
+        <v>911</v>
       </c>
       <c r="B16" t="s">
-        <v>932</v>
+        <v>913</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="D16" t="s">
         <v>111</v>
@@ -8749,13 +8797,13 @@
     </row>
     <row r="17" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>931</v>
+        <v>915</v>
       </c>
       <c r="B17" t="s">
-        <v>933</v>
+        <v>914</v>
       </c>
       <c r="C17" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>111</v>
@@ -8763,10 +8811,10 @@
     </row>
     <row r="18" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>918</v>
+        <v>931</v>
       </c>
       <c r="B18" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C18" t="s">
         <v>115</v>
@@ -8777,10 +8825,10 @@
     </row>
     <row r="19" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>918</v>
+        <v>931</v>
       </c>
       <c r="B19" t="s">
-        <v>917</v>
+        <v>933</v>
       </c>
       <c r="C19" t="s">
         <v>358</v>
@@ -8791,10 +8839,10 @@
     </row>
     <row r="20" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="B20" t="s">
-        <v>430</v>
+        <v>935</v>
       </c>
       <c r="C20" t="s">
         <v>115</v>
@@ -8805,10 +8853,10 @@
     </row>
     <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="B21" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="C21" t="s">
         <v>358</v>
@@ -8822,10 +8870,10 @@
         <v>921</v>
       </c>
       <c r="B22" t="s">
-        <v>934</v>
+        <v>430</v>
       </c>
       <c r="C22" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
         <v>111</v>
@@ -8833,13 +8881,13 @@
     </row>
     <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="B23" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="D23" t="s">
         <v>111</v>
@@ -8847,20 +8895,104 @@
     </row>
     <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="B24" t="s">
-        <v>928</v>
+        <v>934</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>358</v>
       </c>
       <c r="D24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+    <row r="25" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>925</v>
+      </c>
+      <c r="B25" t="s">
+        <v>923</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>929</v>
+      </c>
+      <c r="B26" t="s">
+        <v>928</v>
+      </c>
+      <c r="C26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>967</v>
+      </c>
+      <c r="B27" t="s">
+        <v>973</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>967</v>
+      </c>
+      <c r="B28" t="s">
+        <v>974</v>
+      </c>
+      <c r="C28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>967</v>
+      </c>
+      <c r="B29" t="s">
+        <v>975</v>
+      </c>
+      <c r="C29" t="s">
+        <v>358</v>
+      </c>
+      <c r="D29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>967</v>
+      </c>
+      <c r="B30" t="s">
+        <v>976</v>
+      </c>
+      <c r="C30" t="s">
+        <v>358</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
         <v>863</v>
       </c>
     </row>
@@ -9017,10 +9149,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD56566"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9120,13 +9252,358 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>863</v>
+        <v>128</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>964</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>965</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>966</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>968</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>969</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>970</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>971</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>972</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>862</v>
       </c>
     </row>
@@ -10896,7 +11373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -11114,10 +11591,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131:XFD135"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156:XFD158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15231,19 +15708,19 @@
     </row>
     <row r="109" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
-        <v>794</v>
+        <v>981</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>795</v>
+        <v>969</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D109" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>432</v>
+        <v>982</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>678</v>
@@ -15269,10 +15746,10 @@
     </row>
     <row r="110" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C110" s="12" t="s">
         <v>723</v>
@@ -15281,7 +15758,7 @@
         <v>2</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F110" s="12" t="s">
         <v>678</v>
@@ -15307,19 +15784,19 @@
     </row>
     <row r="111" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>327</v>
+        <v>797</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D111" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>639</v>
+        <v>431</v>
       </c>
       <c r="F111" s="12" t="s">
         <v>678</v>
@@ -15345,10 +15822,10 @@
     </row>
     <row r="112" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
-        <v>329</v>
+        <v>798</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>677</v>
@@ -15357,7 +15834,7 @@
         <v>3</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>437</v>
+        <v>639</v>
       </c>
       <c r="F112" s="12" t="s">
         <v>678</v>
@@ -15383,10 +15860,10 @@
     </row>
     <row r="113" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
-        <v>799</v>
+        <v>329</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>677</v>
@@ -15395,7 +15872,7 @@
         <v>3</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>642</v>
+        <v>437</v>
       </c>
       <c r="F113" s="12" t="s">
         <v>678</v>
@@ -15421,10 +15898,10 @@
     </row>
     <row r="114" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>677</v>
@@ -15433,7 +15910,7 @@
         <v>3</v>
       </c>
       <c r="E114" s="12" t="s">
-        <v>801</v>
+        <v>642</v>
       </c>
       <c r="F114" s="12" t="s">
         <v>678</v>
@@ -15459,10 +15936,10 @@
     </row>
     <row r="115" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="s">
-        <v>330</v>
+        <v>800</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>677</v>
@@ -15471,7 +15948,7 @@
         <v>3</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>438</v>
+        <v>801</v>
       </c>
       <c r="F115" s="12" t="s">
         <v>678</v>
@@ -15497,10 +15974,10 @@
     </row>
     <row r="116" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="s">
-        <v>802</v>
+        <v>330</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>677</v>
@@ -15509,7 +15986,7 @@
         <v>3</v>
       </c>
       <c r="E116" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F116" s="12" t="s">
         <v>678</v>
@@ -15535,10 +16012,10 @@
     </row>
     <row r="117" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>677</v>
@@ -15547,7 +16024,7 @@
         <v>3</v>
       </c>
       <c r="E117" s="12" t="s">
-        <v>643</v>
+        <v>439</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>678</v>
@@ -15573,10 +16050,10 @@
     </row>
     <row r="118" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
-        <v>331</v>
+        <v>803</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>677</v>
@@ -15585,7 +16062,7 @@
         <v>3</v>
       </c>
       <c r="E118" s="12" t="s">
-        <v>440</v>
+        <v>643</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>678</v>
@@ -15611,10 +16088,10 @@
     </row>
     <row r="119" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
-        <v>804</v>
+        <v>331</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>677</v>
@@ -15623,7 +16100,7 @@
         <v>3</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>678</v>
@@ -15649,10 +16126,10 @@
     </row>
     <row r="120" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>677</v>
@@ -15661,7 +16138,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>678</v>
@@ -15687,10 +16164,10 @@
     </row>
     <row r="121" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C121" s="12" t="s">
         <v>677</v>
@@ -15699,7 +16176,7 @@
         <v>3</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F121" s="12" t="s">
         <v>678</v>
@@ -15725,10 +16202,10 @@
     </row>
     <row r="122" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>677</v>
@@ -15737,7 +16214,7 @@
         <v>3</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>644</v>
+        <v>443</v>
       </c>
       <c r="F122" s="12" t="s">
         <v>678</v>
@@ -15763,10 +16240,10 @@
     </row>
     <row r="123" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
-        <v>345</v>
+        <v>807</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C123" s="12" t="s">
         <v>677</v>
@@ -15775,7 +16252,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="12" t="s">
-        <v>444</v>
+        <v>644</v>
       </c>
       <c r="F123" s="12" t="s">
         <v>678</v>
@@ -15801,10 +16278,10 @@
     </row>
     <row r="124" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
-        <v>808</v>
+        <v>345</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>677</v>
@@ -15813,7 +16290,7 @@
         <v>3</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>476</v>
+        <v>444</v>
       </c>
       <c r="F124" s="12" t="s">
         <v>678</v>
@@ -15839,10 +16316,10 @@
     </row>
     <row r="125" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>677</v>
@@ -15851,7 +16328,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="12" t="s">
-        <v>645</v>
+        <v>476</v>
       </c>
       <c r="F125" s="12" t="s">
         <v>678</v>
@@ -15877,10 +16354,10 @@
     </row>
     <row r="126" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>677</v>
@@ -15889,7 +16366,7 @@
         <v>3</v>
       </c>
       <c r="E126" s="12" t="s">
-        <v>445</v>
+        <v>645</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>678</v>
@@ -15915,10 +16392,10 @@
     </row>
     <row r="127" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>231</v>
+        <v>346</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>677</v>
@@ -15927,7 +16404,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="12" t="s">
-        <v>646</v>
+        <v>445</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>678</v>
@@ -15953,10 +16430,10 @@
     </row>
     <row r="128" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>344</v>
+        <v>231</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>677</v>
@@ -15965,7 +16442,7 @@
         <v>3</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F128" s="12" t="s">
         <v>678</v>
@@ -15991,19 +16468,19 @@
     </row>
     <row r="129" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>814</v>
+        <v>344</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D129" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E129" s="12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F129" s="12" t="s">
         <v>678</v>
@@ -16029,19 +16506,19 @@
     </row>
     <row r="130" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>256</v>
+        <v>814</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D130" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E130" s="12" t="s">
-        <v>364</v>
+        <v>648</v>
       </c>
       <c r="F130" s="12" t="s">
         <v>678</v>
@@ -16067,10 +16544,10 @@
     </row>
     <row r="131" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="s">
-        <v>944</v>
+        <v>815</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>944</v>
+        <v>256</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>677</v>
@@ -16079,7 +16556,7 @@
         <v>3</v>
       </c>
       <c r="E131" s="12" t="s">
-        <v>945</v>
+        <v>364</v>
       </c>
       <c r="F131" s="12" t="s">
         <v>678</v>
@@ -16105,10 +16582,10 @@
     </row>
     <row r="132" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="12" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="C132" s="12" t="s">
         <v>677</v>
@@ -16117,7 +16594,7 @@
         <v>3</v>
       </c>
       <c r="E132" s="12" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="F132" s="12" t="s">
         <v>678</v>
@@ -16143,10 +16620,10 @@
     </row>
     <row r="133" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>677</v>
@@ -16155,7 +16632,7 @@
         <v>3</v>
       </c>
       <c r="E133" s="12" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="F133" s="12" t="s">
         <v>678</v>
@@ -16181,10 +16658,10 @@
     </row>
     <row r="134" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="C134" s="12" t="s">
         <v>677</v>
@@ -16193,7 +16670,7 @@
         <v>3</v>
       </c>
       <c r="E134" s="12" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="F134" s="12" t="s">
         <v>678</v>
@@ -16219,10 +16696,10 @@
     </row>
     <row r="135" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="12" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="C135" s="12" t="s">
         <v>677</v>
@@ -16231,7 +16708,7 @@
         <v>3</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="F135" s="12" t="s">
         <v>678</v>
@@ -16257,19 +16734,19 @@
     </row>
     <row r="136" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="12" t="s">
-        <v>837</v>
+        <v>955</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>505</v>
+        <v>956</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D136" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>652</v>
+        <v>957</v>
       </c>
       <c r="F136" s="12" t="s">
         <v>678</v>
@@ -16295,19 +16772,19 @@
     </row>
     <row r="137" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="12" t="s">
-        <v>821</v>
+        <v>979</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>822</v>
+        <v>968</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>723</v>
+        <v>677</v>
       </c>
       <c r="D137" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E137" s="12" t="s">
-        <v>649</v>
+        <v>980</v>
       </c>
       <c r="F137" s="12" t="s">
         <v>678</v>
@@ -16333,10 +16810,10 @@
     </row>
     <row r="138" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>723</v>
@@ -16345,65 +16822,65 @@
         <v>2</v>
       </c>
       <c r="E138" s="12" t="s">
+        <v>649</v>
+      </c>
+      <c r="F138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K138" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L138" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="12" t="s">
+        <v>823</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>824</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="D139" s="12">
+        <v>2</v>
+      </c>
+      <c r="E139" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="F138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K138" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L138" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A139" s="17" t="s">
-        <v>825</v>
-      </c>
-      <c r="B139" s="17" t="s">
-        <v>826</v>
-      </c>
-      <c r="C139" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="D139" s="17">
-        <v>2</v>
-      </c>
-      <c r="E139" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="F139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="G139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="H139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K139" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L139" s="17" t="s">
+      <c r="F139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K139" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L139" s="12" t="s">
         <v>678</v>
       </c>
     </row>
@@ -16412,7 +16889,7 @@
         <v>825</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C140" s="17" t="s">
         <v>723</v>
@@ -16427,7 +16904,7 @@
         <v>678</v>
       </c>
       <c r="G140" s="17" t="s">
-        <v>816</v>
+        <v>678</v>
       </c>
       <c r="H140" s="17" t="s">
         <v>678</v>
@@ -16450,7 +16927,7 @@
         <v>825</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C141" s="17" t="s">
         <v>723</v>
@@ -16465,7 +16942,7 @@
         <v>678</v>
       </c>
       <c r="G141" s="17" t="s">
-        <v>478</v>
+        <v>816</v>
       </c>
       <c r="H141" s="17" t="s">
         <v>678</v>
@@ -16488,7 +16965,7 @@
         <v>825</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C142" s="17" t="s">
         <v>723</v>
@@ -16503,7 +16980,7 @@
         <v>678</v>
       </c>
       <c r="G142" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H142" s="17" t="s">
         <v>678</v>
@@ -16526,7 +17003,7 @@
         <v>825</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C143" s="17" t="s">
         <v>723</v>
@@ -16541,7 +17018,7 @@
         <v>678</v>
       </c>
       <c r="G143" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H143" s="17" t="s">
         <v>678</v>
@@ -16564,7 +17041,7 @@
         <v>825</v>
       </c>
       <c r="B144" s="17" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C144" s="17" t="s">
         <v>723</v>
@@ -16579,7 +17056,7 @@
         <v>678</v>
       </c>
       <c r="G144" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H144" s="17" t="s">
         <v>678</v>
@@ -16602,7 +17079,7 @@
         <v>825</v>
       </c>
       <c r="B145" s="17" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C145" s="17" t="s">
         <v>723</v>
@@ -16617,7 +17094,7 @@
         <v>678</v>
       </c>
       <c r="G145" s="17" t="s">
-        <v>817</v>
+        <v>481</v>
       </c>
       <c r="H145" s="17" t="s">
         <v>678</v>
@@ -16640,7 +17117,7 @@
         <v>825</v>
       </c>
       <c r="B146" s="17" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C146" s="17" t="s">
         <v>723</v>
@@ -16655,7 +17132,7 @@
         <v>678</v>
       </c>
       <c r="G146" s="17" t="s">
-        <v>477</v>
+        <v>817</v>
       </c>
       <c r="H146" s="17" t="s">
         <v>678</v>
@@ -16678,7 +17155,7 @@
         <v>825</v>
       </c>
       <c r="B147" s="17" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C147" s="17" t="s">
         <v>723</v>
@@ -16693,7 +17170,7 @@
         <v>678</v>
       </c>
       <c r="G147" s="17" t="s">
-        <v>818</v>
+        <v>477</v>
       </c>
       <c r="H147" s="17" t="s">
         <v>678</v>
@@ -16716,7 +17193,7 @@
         <v>825</v>
       </c>
       <c r="B148" s="17" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C148" s="17" t="s">
         <v>723</v>
@@ -16731,7 +17208,7 @@
         <v>678</v>
       </c>
       <c r="G148" s="17" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H148" s="17" t="s">
         <v>678</v>
@@ -16754,7 +17231,7 @@
         <v>825</v>
       </c>
       <c r="B149" s="17" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C149" s="17" t="s">
         <v>723</v>
@@ -16769,77 +17246,77 @@
         <v>678</v>
       </c>
       <c r="G149" s="17" t="s">
+        <v>819</v>
+      </c>
+      <c r="H149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K149" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L149" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A150" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>836</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="D150" s="17">
+        <v>2</v>
+      </c>
+      <c r="E150" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F150" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="G150" s="17" t="s">
         <v>820</v>
       </c>
-      <c r="H149" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="I149" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="J149" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="K149" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="L149" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="B150" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="C150" s="12" t="s">
-        <v>677</v>
-      </c>
-      <c r="D150" s="12">
-        <v>3</v>
-      </c>
-      <c r="E150" s="12" t="s">
-        <v>838</v>
-      </c>
-      <c r="F150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K150" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L150" s="12" t="s">
+      <c r="H150" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="I150" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="J150" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="K150" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L150" s="17" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="151" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="12" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>352</v>
+        <v>505</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>677</v>
+        <v>723</v>
       </c>
       <c r="D151" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>840</v>
+        <v>652</v>
       </c>
       <c r="F151" s="12" t="s">
         <v>678</v>
@@ -16865,10 +17342,10 @@
     </row>
     <row r="152" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
-        <v>841</v>
+        <v>983</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>522</v>
+        <v>970</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>677</v>
@@ -16877,7 +17354,7 @@
         <v>3</v>
       </c>
       <c r="E152" s="12" t="s">
-        <v>842</v>
+        <v>984</v>
       </c>
       <c r="F152" s="12" t="s">
         <v>678</v>
@@ -16888,8 +17365,8 @@
       <c r="H152" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I152" s="12" t="s">
-        <v>678</v>
+      <c r="I152" s="12">
+        <v>2</v>
       </c>
       <c r="J152" s="12" t="s">
         <v>678</v>
@@ -16903,10 +17380,10 @@
     </row>
     <row r="153" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="s">
-        <v>843</v>
+        <v>985</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>356</v>
+        <v>971</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>677</v>
@@ -16915,7 +17392,7 @@
         <v>3</v>
       </c>
       <c r="E153" s="12" t="s">
-        <v>844</v>
+        <v>986</v>
       </c>
       <c r="F153" s="12" t="s">
         <v>678</v>
@@ -16941,10 +17418,10 @@
     </row>
     <row r="154" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="s">
-        <v>845</v>
+        <v>987</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>351</v>
+        <v>972</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>677</v>
@@ -16953,7 +17430,7 @@
         <v>3</v>
       </c>
       <c r="E154" s="12" t="s">
-        <v>846</v>
+        <v>988</v>
       </c>
       <c r="F154" s="12" t="s">
         <v>678</v>
@@ -16964,8 +17441,8 @@
       <c r="H154" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I154" s="12" t="s">
-        <v>678</v>
+      <c r="I154" s="12">
+        <v>1</v>
       </c>
       <c r="J154" s="12" t="s">
         <v>678</v>
@@ -16979,10 +17456,10 @@
     </row>
     <row r="155" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="12" t="s">
-        <v>847</v>
+        <v>989</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>355</v>
+        <v>242</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>677</v>
@@ -16991,7 +17468,7 @@
         <v>3</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>848</v>
+        <v>654</v>
       </c>
       <c r="F155" s="12" t="s">
         <v>678</v>
@@ -17002,14 +17479,14 @@
       <c r="H155" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I155" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J155" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K155" s="12" t="s">
-        <v>678</v>
+      <c r="I155" s="12">
+        <v>1</v>
+      </c>
+      <c r="J155" s="12">
+        <v>15</v>
+      </c>
+      <c r="K155" s="12">
+        <v>45</v>
       </c>
       <c r="L155" s="12" t="s">
         <v>678</v>
@@ -17017,10 +17494,10 @@
     </row>
     <row r="156" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="12" t="s">
-        <v>849</v>
+        <v>990</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>353</v>
+        <v>964</v>
       </c>
       <c r="C156" s="12" t="s">
         <v>677</v>
@@ -17029,38 +17506,380 @@
         <v>3</v>
       </c>
       <c r="E156" s="12" t="s">
+        <v>991</v>
+      </c>
+      <c r="F156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J156" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K156" s="12">
+        <v>1</v>
+      </c>
+      <c r="L156" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="12" t="s">
+        <v>992</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>965</v>
+      </c>
+      <c r="C157" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D157" s="12">
+        <v>3</v>
+      </c>
+      <c r="E157" s="12" t="s">
+        <v>993</v>
+      </c>
+      <c r="F157" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G157" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H157" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I157" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J157" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K157" s="12">
+        <v>1</v>
+      </c>
+      <c r="L157" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="12" t="s">
+        <v>994</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>966</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D158" s="12">
+        <v>3</v>
+      </c>
+      <c r="E158" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="F158" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G158" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H158" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I158" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J158" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K158" s="12">
+        <v>1</v>
+      </c>
+      <c r="L158" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C159" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D159" s="12">
+        <v>3</v>
+      </c>
+      <c r="E159" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="F159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K159" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L159" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C160" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D160" s="12">
+        <v>3</v>
+      </c>
+      <c r="E160" s="12" t="s">
+        <v>840</v>
+      </c>
+      <c r="F160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K160" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L160" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="C161" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D161" s="12">
+        <v>3</v>
+      </c>
+      <c r="E161" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="F161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K161" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L161" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="12" t="s">
+        <v>843</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D162" s="12">
+        <v>3</v>
+      </c>
+      <c r="E162" s="12" t="s">
+        <v>844</v>
+      </c>
+      <c r="F162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K162" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L162" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="12" t="s">
+        <v>845</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="C163" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D163" s="12">
+        <v>3</v>
+      </c>
+      <c r="E163" s="12" t="s">
+        <v>846</v>
+      </c>
+      <c r="F163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K163" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L163" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="C164" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D164" s="12">
+        <v>3</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="F164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K164" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L164" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="B165" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="C165" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D165" s="12">
+        <v>3</v>
+      </c>
+      <c r="E165" s="12" t="s">
         <v>850</v>
       </c>
-      <c r="F156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L156" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A158" s="18" t="s">
+      <c r="F165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L165" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A167" s="18" t="s">
         <v>862</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L158">
-    <sortCondition sortBy="cellColor" ref="A19:A158" dxfId="13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L167">
+    <sortCondition sortBy="cellColor" ref="A19:A167" dxfId="7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -17071,8 +17890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD31"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17726,7 +18545,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D51">
-    <sortCondition sortBy="cellColor" ref="A3:A51" dxfId="12"/>
+    <sortCondition sortBy="cellColor" ref="A3:A51" dxfId="6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17734,9 +18553,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17888,15 +18709,15 @@
         <v>539</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="B14" s="17" t="s">
+    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>378</v>
+      <c r="C14" s="12" t="s">
+        <v>977</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -17904,10 +18725,10 @@
         <v>379</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>540</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -17915,10 +18736,10 @@
         <v>379</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>34</v>
+        <v>569</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>467</v>
+        <v>540</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -17926,21 +18747,21 @@
         <v>379</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>568</v>
+        <v>35</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -17948,10 +18769,10 @@
         <v>396</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -17959,21 +18780,21 @@
         <v>396</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>34</v>
+        <v>569</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>378</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>328</v>
+        <v>396</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>568</v>
+        <v>34</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>434</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -17981,10 +18802,10 @@
         <v>328</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -17992,20 +18813,31 @@
         <v>328</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>882</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
-    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C26">
+    <sortCondition sortBy="cellColor" ref="A2:A26" dxfId="5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update functions and related tests for clinical events to phecode mapping
</commit_message>
<xml_diff>
--- a/inst/extdata/dummy_all_lkps_maps_v3.xlsx
+++ b/inst/extdata/dummy_all_lkps_maps_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alasdair/Documents/phd/r_packages/codemapper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF5310-3424-B140-B251-2C0C3B560CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD6B06A-E5A3-604F-9200-E0AECBCBE0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" tabRatio="959" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="1200" windowWidth="27320" windowHeight="19980" tabRatio="959" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="13" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="1052">
   <si>
     <t>BNF_Presentation_Code</t>
   </si>
@@ -3234,6 +3234,174 @@
   </si>
   <si>
     <t>Neonatal diabetes mellitus</t>
+  </si>
+  <si>
+    <t>XE0Uc</t>
+  </si>
+  <si>
+    <t>O10</t>
+  </si>
+  <si>
+    <t>O11X</t>
+  </si>
+  <si>
+    <t>P000</t>
+  </si>
+  <si>
+    <t>Pre-existing hypertension complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.0</t>
+  </si>
+  <si>
+    <t>O100</t>
+  </si>
+  <si>
+    <t>Pre-existing essential hypertension complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.1</t>
+  </si>
+  <si>
+    <t>O101</t>
+  </si>
+  <si>
+    <t>Pre-existing hypertensive heart disease complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.2</t>
+  </si>
+  <si>
+    <t>O102</t>
+  </si>
+  <si>
+    <t>Pre-existing hypertensive renal disease complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.3</t>
+  </si>
+  <si>
+    <t>O103</t>
+  </si>
+  <si>
+    <t>Pre-existing hypertensive heart and renal disease complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.4</t>
+  </si>
+  <si>
+    <t>O104</t>
+  </si>
+  <si>
+    <t>Pre-existing secondary hypertension complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O10.9</t>
+  </si>
+  <si>
+    <t>O109</t>
+  </si>
+  <si>
+    <t>Unspecified pre-existing hypertension complicating pregnancy, childbirth and the puerperium</t>
+  </si>
+  <si>
+    <t>O11</t>
+  </si>
+  <si>
+    <t>Pre-eclampsia superimposed on chronic hypertension</t>
+  </si>
+  <si>
+    <t>P00</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal conditions that may be unrelated to present pregnancy</t>
+  </si>
+  <si>
+    <t>P00.0</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal hypertensive disorders</t>
+  </si>
+  <si>
+    <t>P00.1</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal renal and urinary tract diseases</t>
+  </si>
+  <si>
+    <t>P00.2</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal infectious and parasitic diseases</t>
+  </si>
+  <si>
+    <t>P00.3</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by other maternal circulatory and respiratory diseases</t>
+  </si>
+  <si>
+    <t>P00.4</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal nutritional disorders</t>
+  </si>
+  <si>
+    <t>P00.5</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by maternal injury</t>
+  </si>
+  <si>
+    <t>P00.6</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by surgical procedure on mother</t>
+  </si>
+  <si>
+    <t>P00.7</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by other medical procedures on mother, not elsewhere classified</t>
+  </si>
+  <si>
+    <t>P00.8</t>
+  </si>
+  <si>
+    <t>P008</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by other maternal conditions</t>
+  </si>
+  <si>
+    <t>P00.9</t>
+  </si>
+  <si>
+    <t>P009</t>
+  </si>
+  <si>
+    <t>Fetus and newborn affected by unspecified maternal condition</t>
   </si>
 </sst>
 </file>
@@ -8556,10 +8724,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8937,10 +9105,10 @@
     </row>
     <row r="27" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>967</v>
+        <v>996</v>
       </c>
       <c r="B27" t="s">
-        <v>973</v>
+        <v>434</v>
       </c>
       <c r="C27" t="s">
         <v>115</v>
@@ -8951,10 +9119,10 @@
     </row>
     <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>967</v>
+        <v>996</v>
       </c>
       <c r="B28" t="s">
-        <v>974</v>
+        <v>435</v>
       </c>
       <c r="C28" t="s">
         <v>358</v>
@@ -8968,10 +9136,10 @@
         <v>967</v>
       </c>
       <c r="B29" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C29" t="s">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
         <v>111</v>
@@ -8982,7 +9150,7 @@
         <v>967</v>
       </c>
       <c r="B30" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C30" t="s">
         <v>358</v>
@@ -8991,8 +9159,36 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+    <row r="31" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>967</v>
+      </c>
+      <c r="B31" t="s">
+        <v>975</v>
+      </c>
+      <c r="C31" t="s">
+        <v>358</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>967</v>
+      </c>
+      <c r="B32" t="s">
+        <v>976</v>
+      </c>
+      <c r="C32" t="s">
+        <v>358</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
         <v>863</v>
       </c>
     </row>
@@ -9149,10 +9345,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9597,13 +9793,174 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>863</v>
+        <v>996</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>997</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>999</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>862</v>
       </c>
     </row>
@@ -11591,10 +11948,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L167"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD158"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164:XFD174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17456,10 +17813,10 @@
     </row>
     <row r="155" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="12" t="s">
-        <v>989</v>
+        <v>997</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>242</v>
+        <v>997</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>677</v>
@@ -17468,7 +17825,7 @@
         <v>3</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>654</v>
+        <v>1000</v>
       </c>
       <c r="F155" s="12" t="s">
         <v>678</v>
@@ -17479,14 +17836,14 @@
       <c r="H155" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I155" s="12">
-        <v>1</v>
-      </c>
-      <c r="J155" s="12">
-        <v>15</v>
-      </c>
-      <c r="K155" s="12">
-        <v>45</v>
+      <c r="I155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J155" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K155" s="12" t="s">
+        <v>678</v>
       </c>
       <c r="L155" s="12" t="s">
         <v>678</v>
@@ -17494,10 +17851,10 @@
     </row>
     <row r="156" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="12" t="s">
-        <v>990</v>
+        <v>1001</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>964</v>
+        <v>1002</v>
       </c>
       <c r="C156" s="12" t="s">
         <v>677</v>
@@ -17506,7 +17863,7 @@
         <v>3</v>
       </c>
       <c r="E156" s="12" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
       <c r="F156" s="12" t="s">
         <v>678</v>
@@ -17517,14 +17874,14 @@
       <c r="H156" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I156" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J156" s="12" t="s">
-        <v>678</v>
+      <c r="I156" s="12">
+        <v>1</v>
+      </c>
+      <c r="J156" s="12">
+        <v>15</v>
       </c>
       <c r="K156" s="12">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L156" s="12" t="s">
         <v>678</v>
@@ -17532,10 +17889,10 @@
     </row>
     <row r="157" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="12" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>965</v>
+        <v>1005</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>677</v>
@@ -17544,7 +17901,7 @@
         <v>3</v>
       </c>
       <c r="E157" s="12" t="s">
-        <v>993</v>
+        <v>1006</v>
       </c>
       <c r="F157" s="12" t="s">
         <v>678</v>
@@ -17555,14 +17912,14 @@
       <c r="H157" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I157" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J157" s="12" t="s">
-        <v>678</v>
+      <c r="I157" s="12">
+        <v>1</v>
+      </c>
+      <c r="J157" s="12">
+        <v>15</v>
       </c>
       <c r="K157" s="12">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L157" s="12" t="s">
         <v>678</v>
@@ -17570,10 +17927,10 @@
     </row>
     <row r="158" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="s">
-        <v>994</v>
+        <v>1007</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>966</v>
+        <v>1008</v>
       </c>
       <c r="C158" s="12" t="s">
         <v>677</v>
@@ -17582,7 +17939,7 @@
         <v>3</v>
       </c>
       <c r="E158" s="12" t="s">
-        <v>995</v>
+        <v>1009</v>
       </c>
       <c r="F158" s="12" t="s">
         <v>678</v>
@@ -17593,14 +17950,14 @@
       <c r="H158" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I158" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J158" s="12" t="s">
-        <v>678</v>
+      <c r="I158" s="12">
+        <v>1</v>
+      </c>
+      <c r="J158" s="12">
+        <v>15</v>
       </c>
       <c r="K158" s="12">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L158" s="12" t="s">
         <v>678</v>
@@ -17608,10 +17965,10 @@
     </row>
     <row r="159" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="12" t="s">
-        <v>354</v>
+        <v>1010</v>
       </c>
       <c r="B159" s="12" t="s">
-        <v>354</v>
+        <v>1011</v>
       </c>
       <c r="C159" s="12" t="s">
         <v>677</v>
@@ -17620,7 +17977,7 @@
         <v>3</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>838</v>
+        <v>1012</v>
       </c>
       <c r="F159" s="12" t="s">
         <v>678</v>
@@ -17631,14 +17988,14 @@
       <c r="H159" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I159" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J159" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K159" s="12" t="s">
-        <v>678</v>
+      <c r="I159" s="12">
+        <v>1</v>
+      </c>
+      <c r="J159" s="12">
+        <v>15</v>
+      </c>
+      <c r="K159" s="12">
+        <v>45</v>
       </c>
       <c r="L159" s="12" t="s">
         <v>678</v>
@@ -17646,10 +18003,10 @@
     </row>
     <row r="160" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
-        <v>839</v>
+        <v>1013</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>352</v>
+        <v>1014</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>677</v>
@@ -17658,7 +18015,7 @@
         <v>3</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>840</v>
+        <v>1015</v>
       </c>
       <c r="F160" s="12" t="s">
         <v>678</v>
@@ -17669,14 +18026,14 @@
       <c r="H160" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I160" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J160" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K160" s="12" t="s">
-        <v>678</v>
+      <c r="I160" s="12">
+        <v>1</v>
+      </c>
+      <c r="J160" s="12">
+        <v>15</v>
+      </c>
+      <c r="K160" s="12">
+        <v>45</v>
       </c>
       <c r="L160" s="12" t="s">
         <v>678</v>
@@ -17684,10 +18041,10 @@
     </row>
     <row r="161" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="12" t="s">
-        <v>841</v>
+        <v>1016</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>522</v>
+        <v>1017</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>677</v>
@@ -17696,7 +18053,7 @@
         <v>3</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>842</v>
+        <v>1018</v>
       </c>
       <c r="F161" s="12" t="s">
         <v>678</v>
@@ -17707,14 +18064,14 @@
       <c r="H161" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I161" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J161" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K161" s="12" t="s">
-        <v>678</v>
+      <c r="I161" s="12">
+        <v>1</v>
+      </c>
+      <c r="J161" s="12">
+        <v>15</v>
+      </c>
+      <c r="K161" s="12">
+        <v>45</v>
       </c>
       <c r="L161" s="12" t="s">
         <v>678</v>
@@ -17722,10 +18079,10 @@
     </row>
     <row r="162" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="12" t="s">
-        <v>843</v>
+        <v>1019</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>356</v>
+        <v>998</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>677</v>
@@ -17734,7 +18091,7 @@
         <v>3</v>
       </c>
       <c r="E162" s="12" t="s">
-        <v>844</v>
+        <v>1020</v>
       </c>
       <c r="F162" s="12" t="s">
         <v>678</v>
@@ -17745,14 +18102,14 @@
       <c r="H162" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I162" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J162" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K162" s="12" t="s">
-        <v>678</v>
+      <c r="I162" s="12">
+        <v>1</v>
+      </c>
+      <c r="J162" s="12">
+        <v>15</v>
+      </c>
+      <c r="K162" s="12">
+        <v>45</v>
       </c>
       <c r="L162" s="12" t="s">
         <v>678</v>
@@ -17760,10 +18117,10 @@
     </row>
     <row r="163" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="12" t="s">
-        <v>845</v>
+        <v>989</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>351</v>
+        <v>242</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>677</v>
@@ -17772,7 +18129,7 @@
         <v>3</v>
       </c>
       <c r="E163" s="12" t="s">
-        <v>846</v>
+        <v>654</v>
       </c>
       <c r="F163" s="12" t="s">
         <v>678</v>
@@ -17783,14 +18140,14 @@
       <c r="H163" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="I163" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J163" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K163" s="12" t="s">
-        <v>678</v>
+      <c r="I163" s="12">
+        <v>1</v>
+      </c>
+      <c r="J163" s="12">
+        <v>15</v>
+      </c>
+      <c r="K163" s="12">
+        <v>45</v>
       </c>
       <c r="L163" s="12" t="s">
         <v>678</v>
@@ -17798,10 +18155,10 @@
     </row>
     <row r="164" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="12" t="s">
-        <v>847</v>
+        <v>1021</v>
       </c>
       <c r="B164" s="12" t="s">
-        <v>355</v>
+        <v>1021</v>
       </c>
       <c r="C164" s="12" t="s">
         <v>677</v>
@@ -17810,7 +18167,7 @@
         <v>3</v>
       </c>
       <c r="E164" s="12" t="s">
-        <v>848</v>
+        <v>1022</v>
       </c>
       <c r="F164" s="12" t="s">
         <v>678</v>
@@ -17836,10 +18193,10 @@
     </row>
     <row r="165" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="12" t="s">
-        <v>849</v>
+        <v>1023</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>353</v>
+        <v>999</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>677</v>
@@ -17848,38 +18205,760 @@
         <v>3</v>
       </c>
       <c r="E165" s="12" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J165" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K165" s="12">
+        <v>1</v>
+      </c>
+      <c r="L165" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="12" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C166" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D166" s="12">
+        <v>3</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F166" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G166" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H166" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I166" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J166" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K166" s="12">
+        <v>1</v>
+      </c>
+      <c r="L166" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="12" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B167" s="12" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C167" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D167" s="12">
+        <v>3</v>
+      </c>
+      <c r="E167" s="12" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F167" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G167" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H167" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I167" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J167" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K167" s="12">
+        <v>1</v>
+      </c>
+      <c r="L167" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="12" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D168" s="12">
+        <v>3</v>
+      </c>
+      <c r="E168" s="12" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F168" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G168" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H168" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I168" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J168" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K168" s="12">
+        <v>1</v>
+      </c>
+      <c r="L168" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B169" s="12" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C169" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D169" s="12">
+        <v>3</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F169" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G169" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H169" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I169" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J169" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K169" s="12">
+        <v>1</v>
+      </c>
+      <c r="L169" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="12" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B170" s="12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C170" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D170" s="12">
+        <v>3</v>
+      </c>
+      <c r="E170" s="12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F170" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G170" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H170" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I170" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J170" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K170" s="12">
+        <v>1</v>
+      </c>
+      <c r="L170" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="12" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B171" s="12" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C171" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D171" s="12">
+        <v>3</v>
+      </c>
+      <c r="E171" s="12" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F171" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G171" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H171" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I171" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J171" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K171" s="12">
+        <v>1</v>
+      </c>
+      <c r="L171" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B172" s="12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D172" s="12">
+        <v>3</v>
+      </c>
+      <c r="E172" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F172" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G172" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H172" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I172" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J172" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K172" s="12">
+        <v>1</v>
+      </c>
+      <c r="L172" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="12" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B173" s="12" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C173" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D173" s="12">
+        <v>3</v>
+      </c>
+      <c r="E173" s="12" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F173" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G173" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H173" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I173" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J173" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K173" s="12">
+        <v>1</v>
+      </c>
+      <c r="L173" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="12" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B174" s="12" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D174" s="12">
+        <v>3</v>
+      </c>
+      <c r="E174" s="12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F174" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G174" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H174" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I174" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J174" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K174" s="12">
+        <v>1</v>
+      </c>
+      <c r="L174" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>964</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D175" s="12">
+        <v>3</v>
+      </c>
+      <c r="E175" s="12" t="s">
+        <v>991</v>
+      </c>
+      <c r="F175" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G175" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H175" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I175" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J175" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K175" s="12">
+        <v>1</v>
+      </c>
+      <c r="L175" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="12" t="s">
+        <v>992</v>
+      </c>
+      <c r="B176" s="12" t="s">
+        <v>965</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D176" s="12">
+        <v>3</v>
+      </c>
+      <c r="E176" s="12" t="s">
+        <v>993</v>
+      </c>
+      <c r="F176" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G176" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H176" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I176" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J176" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K176" s="12">
+        <v>1</v>
+      </c>
+      <c r="L176" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="12" t="s">
+        <v>994</v>
+      </c>
+      <c r="B177" s="12" t="s">
+        <v>966</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D177" s="12">
+        <v>3</v>
+      </c>
+      <c r="E177" s="12" t="s">
+        <v>995</v>
+      </c>
+      <c r="F177" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G177" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H177" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I177" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J177" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K177" s="12">
+        <v>1</v>
+      </c>
+      <c r="L177" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C178" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D178" s="12">
+        <v>3</v>
+      </c>
+      <c r="E178" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="F178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L178" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B179" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C179" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D179" s="12">
+        <v>3</v>
+      </c>
+      <c r="E179" s="12" t="s">
+        <v>840</v>
+      </c>
+      <c r="F179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L179" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D180" s="12">
+        <v>3</v>
+      </c>
+      <c r="E180" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="F180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L180" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="12" t="s">
+        <v>843</v>
+      </c>
+      <c r="B181" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="C181" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D181" s="12">
+        <v>3</v>
+      </c>
+      <c r="E181" s="12" t="s">
+        <v>844</v>
+      </c>
+      <c r="F181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L181" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="12" t="s">
+        <v>845</v>
+      </c>
+      <c r="B182" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D182" s="12">
+        <v>3</v>
+      </c>
+      <c r="E182" s="12" t="s">
+        <v>846</v>
+      </c>
+      <c r="F182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K182" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L182" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="B183" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D183" s="12">
+        <v>3</v>
+      </c>
+      <c r="E183" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="F183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K183" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L183" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="B184" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D184" s="12">
+        <v>3</v>
+      </c>
+      <c r="E184" s="12" t="s">
         <v>850</v>
       </c>
-      <c r="F165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="G165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="I165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="J165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="K165" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="L165" s="12" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A167" s="18" t="s">
+      <c r="F184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="G184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="J184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="K184" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="L184" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A186" s="18" t="s">
         <v>862</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L167">
-    <sortCondition sortBy="cellColor" ref="A19:A167" dxfId="7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L186">
+    <sortCondition sortBy="cellColor" ref="A19:A186" dxfId="7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>